<commit_message>
Perubahan Data Input dan Inference Cell
</commit_message>
<xml_diff>
--- a/datainput.xlsx
+++ b/datainput.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22DB957E-29E5-49AC-8487-04E6E98066BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ADC295-AF9B-4DE3-B02C-0CFFF5D197DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2C917602-9D81-45FD-9BED-B6F085321F49}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Age</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>YearsWithCurrManager</t>
+  </si>
+  <si>
+    <t>Travel_Frequently</t>
+  </si>
+  <si>
+    <t>Human Resources</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -144,8 +162,8 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,22 +193,598 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="JetBrains Mono"/>
+        <family val="3"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -208,40 +802,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7DAA333-C9F1-4914-8A45-130AAE3DB965}" name="Table1" displayName="Table1" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:AE2" xr:uid="{B7DAA333-C9F1-4914-8A45-130AAE3DB965}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F860EF6-E4D2-4FAC-952A-E31C0B707850}" name="Table1" displayName="Table1" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:AE2" xr:uid="{1F860EF6-E4D2-4FAC-952A-E31C0B707850}"/>
   <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{0CC5D3C2-53C2-4463-814F-27C910EC2A48}" name="Age"/>
-    <tableColumn id="2" xr3:uid="{71C61CAC-1EA9-4802-A382-32D3C83A11CD}" name="BusinessTravel"/>
-    <tableColumn id="3" xr3:uid="{345D1554-6A2D-46D6-8DB6-38A9BCFEECF9}" name="DailyRate"/>
-    <tableColumn id="4" xr3:uid="{BFC30B2A-0D53-4718-84E1-2EC320402397}" name="Department"/>
-    <tableColumn id="5" xr3:uid="{890C975D-C7E6-47AE-8DE5-FC5A895425F2}" name="DistanceFromHome"/>
-    <tableColumn id="6" xr3:uid="{DB5A2E09-7858-48DC-B0A7-9C6AD163C5CE}" name="Education"/>
-    <tableColumn id="7" xr3:uid="{3EDE9815-FC30-4E6C-AAF1-7538533261EC}" name="EducationField"/>
-    <tableColumn id="8" xr3:uid="{16D81543-D9DA-49AA-93A9-985DC3E408E4}" name="EnvironmentSatisfaction"/>
-    <tableColumn id="9" xr3:uid="{F717D3CA-8801-4C6B-BCB3-F079EE548AB5}" name="Gender"/>
-    <tableColumn id="10" xr3:uid="{2C2F6378-1E2F-4875-9C9B-5CEC48321C6C}" name="HourlyRate"/>
-    <tableColumn id="11" xr3:uid="{A1C7B4B5-F39B-4505-BDD1-F45F3600184D}" name="JobInvolvement"/>
-    <tableColumn id="12" xr3:uid="{030D15B1-97C1-4730-8811-2400F06408C8}" name="JobLevel"/>
-    <tableColumn id="13" xr3:uid="{05A363C2-B476-4E27-A468-6A328466BDCA}" name="JobRole"/>
-    <tableColumn id="14" xr3:uid="{19D6C0B3-0C4D-43AF-95C9-900A3E03AEE6}" name="JobSatisfaction"/>
-    <tableColumn id="15" xr3:uid="{54294317-0A0F-4889-8D26-E449F1B400AF}" name="MaritalStatus"/>
-    <tableColumn id="16" xr3:uid="{70B6D060-91D3-4E89-B6E1-1E83AC2096BC}" name="MonthlyIncome"/>
-    <tableColumn id="17" xr3:uid="{780E023A-2184-453F-925B-5F4EF397FCCF}" name="MonthlyRate"/>
-    <tableColumn id="18" xr3:uid="{4376A00D-67C7-4ABE-9072-B3F55702E61D}" name="NumCompaniesWorked"/>
-    <tableColumn id="19" xr3:uid="{64CF560F-3765-4492-864A-95814A77B475}" name="OverTime"/>
-    <tableColumn id="20" xr3:uid="{2099BC49-121A-4DCC-ABD5-0F0D9F933534}" name="PercentSalaryHike"/>
-    <tableColumn id="21" xr3:uid="{2363F4DB-9407-44A0-BA2F-24AEE77CC088}" name="PerformanceRating"/>
-    <tableColumn id="22" xr3:uid="{29DEBB0D-F0F8-4650-8079-FC79F51C6701}" name="RelationshipSatisfaction"/>
-    <tableColumn id="23" xr3:uid="{DD205D1E-5453-4154-A64B-0585A9F6F917}" name="StandardHours"/>
-    <tableColumn id="24" xr3:uid="{4CAC0006-6121-46C2-9074-B81025BC944B}" name="StockOptionLevel"/>
-    <tableColumn id="25" xr3:uid="{B044B6B8-BB32-4482-A50A-2B2F4B4A88BF}" name="TotalWorkingYears"/>
-    <tableColumn id="26" xr3:uid="{B8B60452-7761-4D5A-B0AA-2DCFB104B950}" name="TrainingTimesLastYear"/>
-    <tableColumn id="27" xr3:uid="{B5CF6434-C12F-4303-B777-83523DB30522}" name="WorkLifeBalance"/>
-    <tableColumn id="28" xr3:uid="{B5F8204A-3E00-4C44-8690-FE1C45D896FE}" name="YearsAtCompany"/>
-    <tableColumn id="29" xr3:uid="{C0CAAAC0-AB76-4589-90E1-9D198DFF6E9C}" name="YearsInCurrentRole"/>
-    <tableColumn id="30" xr3:uid="{E95E1EDC-1B54-46F9-99EB-CD57A1B9D8C4}" name="YearsSinceLastPromotion"/>
-    <tableColumn id="31" xr3:uid="{20EBF83A-C02D-4934-99ED-C3A2739A04CC}" name="YearsWithCurrManager"/>
+    <tableColumn id="2" xr3:uid="{98C5F77B-9DCC-4BF4-AE43-B84CF150EB2A}" name="Age" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{B22D0227-ECEE-4765-BE04-3DB95B982523}" name="BusinessTravel" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{E96F52F7-5A46-45B0-A238-DEDEE535298B}" name="DailyRate" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{D08177B2-75EB-4BCE-8C2A-BFB56D51798D}" name="Department" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{548B6238-0422-4677-8F43-8E58F42C3D35}" name="DistanceFromHome" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{35587CFD-FB44-43F9-85C5-507DFA291ABF}" name="Education" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{0D68BB12-30FF-4430-9485-C5D7C595552A}" name="EducationField" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{D31BBB39-D9D4-4C6B-9840-EAD6037A28F3}" name="EnvironmentSatisfaction" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{FD2387B5-7846-47D5-A407-EAAEAB681B76}" name="Gender" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{F8E19CAE-141F-4A2C-8D33-5196F632327D}" name="HourlyRate" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{54BE0C99-12AE-4DC4-AADF-04D19C56ADFE}" name="JobInvolvement" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{6A4B6FF4-B995-422C-8759-CF7501A621AF}" name="JobLevel" dataDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{5CF060B9-BC90-4C64-A7E2-52D3072A9BDE}" name="JobRole" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{CEF4BD28-C3B7-4A7C-8846-D24E6C71CDA4}" name="JobSatisfaction" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{24C6682B-CA8D-4A3C-95B8-6A846BD9A835}" name="MaritalStatus" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{6BAE23B9-C08F-4CED-8CDC-928813F720F1}" name="MonthlyIncome" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{CB3B822C-4750-4DA0-9F4C-06A384196678}" name="MonthlyRate" dataDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{038AFC10-7E33-4ABB-82D2-06413D057882}" name="NumCompaniesWorked" dataDxfId="13"/>
+    <tableColumn id="23" xr3:uid="{E2AEA7B0-7702-474E-A5F6-CA1AE71ADEED}" name="OverTime" dataDxfId="12"/>
+    <tableColumn id="24" xr3:uid="{A479A1F3-AC54-4983-ADF4-9E9F73122F74}" name="PercentSalaryHike" dataDxfId="11"/>
+    <tableColumn id="25" xr3:uid="{8D39C672-7114-464B-8CDD-D2E48EF8548D}" name="PerformanceRating" dataDxfId="10"/>
+    <tableColumn id="26" xr3:uid="{09A307D4-4D06-4934-942E-98EDF6BBE106}" name="RelationshipSatisfaction" dataDxfId="9"/>
+    <tableColumn id="27" xr3:uid="{9867E383-4502-4261-AD24-0CBA53355CEA}" name="StandardHours" dataDxfId="8"/>
+    <tableColumn id="28" xr3:uid="{17D3ECA5-B716-4ED6-BEA6-22752B22FA42}" name="StockOptionLevel" dataDxfId="7"/>
+    <tableColumn id="29" xr3:uid="{F8A2C452-643D-467C-B69C-36CB8A801F6C}" name="TotalWorkingYears" dataDxfId="6"/>
+    <tableColumn id="30" xr3:uid="{4DA24FBF-F277-4E38-9AC1-5C67C470085D}" name="TrainingTimesLastYear" dataDxfId="5"/>
+    <tableColumn id="31" xr3:uid="{4036DAB4-9D7F-4DA9-A645-AA35668E81FE}" name="WorkLifeBalance" dataDxfId="4"/>
+    <tableColumn id="32" xr3:uid="{5F99C755-4436-497A-95FF-56C75B42CF8E}" name="YearsAtCompany" dataDxfId="3"/>
+    <tableColumn id="33" xr3:uid="{A940F7ED-147B-4D82-9CF8-C2620BCFDBDE}" name="YearsInCurrentRole" dataDxfId="2"/>
+    <tableColumn id="34" xr3:uid="{1A097BAD-DB1D-4D17-8AA0-73D81E194262}" name="YearsSinceLastPromotion" dataDxfId="1"/>
+    <tableColumn id="35" xr3:uid="{D72C9794-7D76-4737-8D30-44F61059DE9E}" name="YearsWithCurrManager" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,45 +1137,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E2E005-8368-4BC9-A97D-00AF1E0BAFE3}">
-  <dimension ref="A1:AE1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3D15D7-5639-4799-95F3-B90A220AD24D}">
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.08984375" customWidth="1"/>
-    <col min="11" max="11" width="14.1796875" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" customWidth="1"/>
-    <col min="16" max="16" width="13.90625" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="19.90625" customWidth="1"/>
-    <col min="19" max="19" width="10.1796875" customWidth="1"/>
-    <col min="20" max="20" width="16.26953125" customWidth="1"/>
-    <col min="21" max="21" width="16.54296875" customWidth="1"/>
-    <col min="22" max="22" width="20.36328125" customWidth="1"/>
-    <col min="23" max="23" width="13.54296875" customWidth="1"/>
-    <col min="24" max="24" width="15.81640625" customWidth="1"/>
-    <col min="25" max="25" width="17.08984375" customWidth="1"/>
-    <col min="26" max="26" width="19.90625" customWidth="1"/>
-    <col min="27" max="28" width="15.54296875" customWidth="1"/>
-    <col min="29" max="29" width="17.26953125" customWidth="1"/>
-    <col min="30" max="30" width="21.54296875" customWidth="1"/>
-    <col min="31" max="31" width="20.08984375" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="27.90625" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" customWidth="1"/>
+    <col min="11" max="11" width="18.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" customWidth="1"/>
+    <col min="15" max="16" width="17" customWidth="1"/>
+    <col min="17" max="17" width="14.81640625" customWidth="1"/>
+    <col min="18" max="18" width="22.453125" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" customWidth="1"/>
+    <col min="20" max="21" width="21.36328125" customWidth="1"/>
+    <col min="22" max="22" width="29" customWidth="1"/>
+    <col min="23" max="23" width="17" customWidth="1"/>
+    <col min="24" max="24" width="20.26953125" customWidth="1"/>
+    <col min="25" max="25" width="21.36328125" customWidth="1"/>
+    <col min="26" max="26" width="25.7265625" customWidth="1"/>
+    <col min="27" max="27" width="19.1796875" customWidth="1"/>
+    <col min="28" max="28" width="18.08984375" customWidth="1"/>
+    <col min="29" max="29" width="22.453125" customWidth="1"/>
+    <col min="30" max="30" width="27.90625" customWidth="1"/>
+    <col min="31" max="31" width="24.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
@@ -677,6 +1269,101 @@
       </c>
       <c r="AE1" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1444</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="1">
+        <v>88</v>
+      </c>
+      <c r="K2" s="1">
+        <v>3</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2991</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>5224</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="1">
+        <v>11</v>
+      </c>
+      <c r="U2" s="1">
+        <v>3</v>
+      </c>
+      <c r="V2" s="1">
+        <v>2</v>
+      </c>
+      <c r="W2" s="1">
+        <v>80</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>